<commit_message>
Added the ability to store all the movies in an excel sheet an then send it to a specific email
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -14,7 +14,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <x:si>
+    <x:t>TAYLOR SWIFT | THE ERAS TOUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 HR 48 MIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PG13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Released Oct 13, 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TAYLOR SWIFT | THE ERAS TOUR: Private Theatre Rental for up to 40 Guests</x:t>
+  </x:si>
   <x:si>
     <x:t>The Exorcist: Believer</x:t>
   </x:si>
@@ -47,24 +62,21 @@
     <x:t>1 HR 58 MIN</x:t>
   </x:si>
   <x:si>
+    <x:t>The Nun II</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 HR 50 MIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Released Sep 8, 2023</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Creator</x:t>
   </x:si>
   <x:si>
     <x:t>2 HR 13 MIN</x:t>
   </x:si>
   <x:si>
-    <x:t>PG13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Nun II</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 50 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Released Sep 8, 2023</x:t>
-  </x:si>
-  <x:si>
     <x:t>Dumb Money</x:t>
   </x:si>
   <x:si>
@@ -89,85 +101,67 @@
     <x:t>Released Sep 1, 2023</x:t>
   </x:si>
   <x:si>
+    <x:t>Barbie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 HR 54 MIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Released Jul 21, 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EXPEND4BLES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Released Sep 22, 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>My Big Fat Greek Wedding 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 HR 32 MIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oppenheimer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 HR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hocus Pocus 30th Anniversary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 HR 36 MIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Under The Skin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Opening Oct 18, 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beetlejuice 35th Anniversary</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Blind</x:t>
   </x:si>
   <x:si>
     <x:t>Released Sep 28, 2023</x:t>
   </x:si>
   <x:si>
-    <x:t>EXPEND4BLES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Released Sep 22, 2023</x:t>
-  </x:si>
-  <x:si>
-    <x:t>My Big Fat Greek Wedding 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 32 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Barbie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 54 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Released Jul 21, 2023</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hocus Pocus 30th Anniversary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 36 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Opening Oct 11, 2023</x:t>
-  </x:si>
-  <x:si>
-    <x:t>It Lives Inside</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 39 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blue Beetle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 HR 7 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Released Aug 18, 2023</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oppenheimer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 HR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Royal Hotel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 HR 31 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Teenage Mutant Ninja Turtles: Mutant Mayhem</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Released Aug 2, 2023</x:t>
+    <x:t>Still Playin' Possum: Music and Memories of George Jones</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Opening Oct 17, 2023</x:t>
   </x:si>
   <x:si>
     <x:t>When Evil Lurks</x:t>
   </x:si>
   <x:si>
     <x:t>1 HR 40 MIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NR</x:t>
   </x:si>
   <x:si>
     <x:t>Stop Making Sense</x:t>
@@ -567,41 +561,41 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>12</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -612,77 +606,77 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
       <x:c r="C7" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
         <x:v>12</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
       <x:c r="A8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s">
+      <x:c r="C8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="A9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="A10" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>27</x:v>
@@ -696,21 +690,21 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>32</x:v>
@@ -724,10 +718,10 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
@@ -735,13 +729,13 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
@@ -752,10 +746,10 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
@@ -763,130 +757,130 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
         <x:v>40</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>